<commit_message>
Adjusted repository contents before paper publication
</commit_message>
<xml_diff>
--- a/vioWithData.xlsx
+++ b/vioWithData.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="23628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="11116"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/93e46a4a03755bf4/Nova IMS/Project/nlp_project/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/93e46a4a03755bf4/Nova IMS/Project/nlp_project/mscProjectDocSimilarity/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="4" documentId="11_D3AA1EDAEC09EAEFA2160B29431CDE7D502A552A" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{F301C384-E088-4DF2-A8D8-600968982006}"/>
+  <xr:revisionPtr revIDLastSave="5" documentId="11_D3AA1EDAEC09EAEFA2160B29431CDE7D502A552A" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{41D5B0DF-8E2D-A046-B908-3FB857B217E1}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="23260" windowHeight="13180" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -475,9 +475,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2007 - 2010">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -515,9 +515,9 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2007 - 2010">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -550,26 +550,9 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -602,26 +585,9 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2007 - 2010">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -797,18 +763,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E51"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
       <selection activeCell="B1" sqref="B1:E51"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="9.5546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.5" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="50.33203125" customWidth="1"/>
     <col min="4" max="4" width="124.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="255.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -822,7 +789,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" s="1">
         <v>539</v>
       </c>
@@ -839,7 +806,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" s="1">
         <v>565</v>
       </c>
@@ -856,7 +823,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" s="1">
         <v>560</v>
       </c>
@@ -873,7 +840,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" s="1">
         <v>276</v>
       </c>
@@ -890,7 +857,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" s="1">
         <v>178</v>
       </c>
@@ -907,7 +874,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" s="1">
         <v>1753</v>
       </c>
@@ -924,7 +891,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8" s="1">
         <v>1771</v>
       </c>
@@ -941,7 +908,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9" s="1">
         <v>43</v>
       </c>
@@ -958,7 +925,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10" s="1">
         <v>1599</v>
       </c>
@@ -975,7 +942,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A11" s="1">
         <v>1370</v>
       </c>
@@ -992,7 +959,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A12" s="1">
         <v>1087</v>
       </c>
@@ -1009,7 +976,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A13" s="1">
         <v>1278</v>
       </c>
@@ -1026,7 +993,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A14" s="1">
         <v>1397</v>
       </c>
@@ -1043,7 +1010,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A15" s="1">
         <v>1266</v>
       </c>
@@ -1060,7 +1027,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A16" s="1">
         <v>1772</v>
       </c>
@@ -1077,7 +1044,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A17" s="1">
         <v>1133</v>
       </c>
@@ -1094,7 +1061,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A18" s="1">
         <v>603</v>
       </c>
@@ -1111,7 +1078,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A19" s="1">
         <v>1754</v>
       </c>
@@ -1128,7 +1095,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A20" s="1">
         <v>1516</v>
       </c>
@@ -1145,7 +1112,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A21" s="1">
         <v>8</v>
       </c>
@@ -1162,7 +1129,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A22" s="1">
         <v>745</v>
       </c>
@@ -1179,7 +1146,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A23" s="1">
         <v>1213</v>
       </c>
@@ -1196,7 +1163,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A24" s="1">
         <v>1294</v>
       </c>
@@ -1213,7 +1180,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A25" s="1">
         <v>731</v>
       </c>
@@ -1230,7 +1197,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A26" s="1">
         <v>1743</v>
       </c>
@@ -1247,7 +1214,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A27" s="1">
         <v>610</v>
       </c>
@@ -1264,7 +1231,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A28" s="1">
         <v>664</v>
       </c>
@@ -1281,7 +1248,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A29" s="1">
         <v>1540</v>
       </c>
@@ -1298,7 +1265,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A30" s="1">
         <v>1848</v>
       </c>
@@ -1315,7 +1282,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A31" s="1">
         <v>1510</v>
       </c>
@@ -1332,7 +1299,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A32" s="1">
         <v>833</v>
       </c>
@@ -1349,7 +1316,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A33" s="1">
         <v>353</v>
       </c>
@@ -1366,7 +1333,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A34" s="1">
         <v>1426</v>
       </c>
@@ -1383,7 +1350,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A35" s="1">
         <v>141</v>
       </c>
@@ -1400,7 +1367,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A36" s="1">
         <v>1371</v>
       </c>
@@ -1417,7 +1384,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A37" s="1">
         <v>395</v>
       </c>
@@ -1434,7 +1401,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A38" s="1">
         <v>211</v>
       </c>
@@ -1451,7 +1418,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A39" s="1">
         <v>1411</v>
       </c>
@@ -1468,7 +1435,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A40" s="1">
         <v>1422</v>
       </c>
@@ -1485,7 +1452,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A41" s="1">
         <v>1565</v>
       </c>
@@ -1502,7 +1469,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A42" s="1">
         <v>118</v>
       </c>
@@ -1519,7 +1486,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A43" s="1">
         <v>991</v>
       </c>
@@ -1536,7 +1503,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A44" s="1">
         <v>1123</v>
       </c>
@@ -1553,7 +1520,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A45" s="1">
         <v>700</v>
       </c>
@@ -1570,7 +1537,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A46" s="1">
         <v>1377</v>
       </c>
@@ -1587,7 +1554,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A47" s="1">
         <v>1725</v>
       </c>
@@ -1604,7 +1571,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A48" s="1">
         <v>1594</v>
       </c>
@@ -1621,7 +1588,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A49" s="1">
         <v>1413</v>
       </c>
@@ -1638,7 +1605,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A50" s="1">
         <v>1005</v>
       </c>
@@ -1655,7 +1622,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A51" s="1">
         <v>1427</v>
       </c>

</xml_diff>